<commit_message>
Files for verification updated
</commit_message>
<xml_diff>
--- a/verification.xlsx
+++ b/verification.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="interval_estimation" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="valori_attesi_maggiori" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t xml:space="preserve">Statistic</t>
   </si>
@@ -64,109 +65,109 @@
     <t xml:space="preserve">Response time normal center</t>
   </si>
   <si>
+    <t xml:space="preserve"> 224.062908 +/- 4.812282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response time premium center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 143.158816 +/- 1.413922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response time reliable center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 458.945732 +/- 26.611969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting time digest center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.363271 +/- 0.005838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting time normal center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 76.828723 +/- 4.738207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting time premium center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23.970745 +/- 1.375199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting time reliable center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 383.926029 +/- 26.391946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service time digest center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.600008 +/- 0.000323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service time normal center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 147.234185 +/- 0.134146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service time premium center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 119.188072 +/- 0.077270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service time reliable center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 75.019703 +/- 0.402554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interarrival time digest center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.864200 +/- 0.000445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interarrival time normal center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.025166 +/- 0.002814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interarrival time premium center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.297737 +/- 0.000806</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interarrival time reliable center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 88.965814 +/- 0.461334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average number of jobs in digest center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.271863 +/- 0.007595</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average number of jobs in normal center</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> 224.062908 +/- 4.812282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response time premium center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 143.158816 +/- 1.413922</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response time reliable center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 458.945732 +/- 26.611969</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waiting time digest center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.363271 +/- 0.005838</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waiting time normal center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 76.828723 +/- 4.738207</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waiting time premium center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 23.970745 +/- 1.375199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waiting time reliable center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 383.926029 +/- 26.391946</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service time digest center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.600008 +/- 0.000323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service time normal center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 147.234185 +/- 0.134146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service time premium center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 119.188072 +/- 0.077270</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service time reliable center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 75.019703 +/- 0.402554</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interarrival time digest center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.864200 +/- 0.000445</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interarrival time normal center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.025166 +/- 0.002814</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interarrival time premium center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.297737 +/- 0.000806</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interarrival time reliable center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 88.965814 +/- 0.461334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average number of jobs in digest center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2.271863 +/- 0.007595</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average number of jobs in normal center</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 74.091398 +/- 1.625701</t>
   </si>
   <si>
-    <t xml:space="preserve">Average number of jobs in premium center</t>
+    <t xml:space="preserve">Average number of jobs in premium centerù</t>
   </si>
   <si>
     <t xml:space="preserve"> 110.327612 +/- 1.130062</t>
@@ -199,13 +200,13 @@
     <t xml:space="preserve">Global response time</t>
   </si>
   <si>
-    <t xml:space="preserve"> 165.793473 +/- 1.765061</t>
+    <t xml:space="preserve">165.793473 +/- 1.765061</t>
   </si>
   <si>
     <t xml:space="preserve">Global Premium response time</t>
   </si>
   <si>
-    <t xml:space="preserve"> 140.174912 +/- 1.353109</t>
+    <t xml:space="preserve">141.137177 +/- 1.397107</t>
   </si>
   <si>
     <t xml:space="preserve">Failure percentage</t>
@@ -327,8 +328,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,13 +357,13 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.06"/>
   </cols>
   <sheetData>
@@ -432,189 +437,193 @@
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="n">
+        <v>232.945742</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>144.375297</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>17</v>
+      <c r="E8" s="0" t="n">
+        <f aca="false">143.158816+1.413922</f>
+        <v>144.572738</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>451.061608</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1.363633</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>85.693088</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>25.183851</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>376.061608</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.6</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>147.252654</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>119.191446</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>75</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">1/(B2/86400)</f>
         <v>0.864</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">TRUNC(1/(B39/86400),6)</f>
         <v>3.026799</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">TRUNC(1/(B40/86400),6)</f>
         <v>1.297199</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">TRUNC(1/(B41/86400),6)</f>
         <v>88.838877</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">TRUNC(1/B18*B6,6)</f>
         <v>2.272723</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>47</v>
@@ -625,7 +634,7 @@
         <v>48</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>49</v>
@@ -683,8 +692,9 @@
       <c r="A29" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>14</v>
+      <c r="B29" s="0" t="n">
+        <f aca="false">TRUNC(B6 + B7*B39/B2 + B8*B40/B2 + B9*B41/B2,6)</f>
+        <v>169.005948</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -694,8 +704,9 @@
       <c r="A30" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>14</v>
+      <c r="B30" s="0" t="n">
+        <f aca="false">TRUNC(B6 + B8*B40/B2 + 148.418018*B37, 6)</f>
+        <v>99.124691</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>61</v>
@@ -717,8 +728,9 @@
       <c r="A32" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>14</v>
+      <c r="B32" s="0" t="n">
+        <f aca="false">TRUNC(B14/B18,6)</f>
+        <v>0.694444</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>65</v>
@@ -728,8 +740,9 @@
       <c r="A33" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>14</v>
+      <c r="B33" s="0" t="n">
+        <f aca="false">TRUNC(B15/(B19*50),6)</f>
+        <v>0.972992</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>67</v>
@@ -739,8 +752,9 @@
       <c r="A34" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>14</v>
+      <c r="B34" s="1" t="n">
+        <f aca="false">TRUNC(B16/(B20*95),6)</f>
+        <v>0.967196</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>69</v>
@@ -750,8 +764,9 @@
       <c r="A35" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>14</v>
+      <c r="B35" s="1" t="n">
+        <f aca="false">TRUNC(B17/(B21),6)</f>
+        <v>0.844224</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>71</v>
@@ -822,4 +837,57 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.51"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>232.945742</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>85.693088</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Pagina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code is almost all commented; fixed verification.xlsx file
</commit_message>
<xml_diff>
--- a/verification.xlsx
+++ b/verification.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
   <si>
     <t xml:space="preserve">Statistic</t>
   </si>
@@ -161,9 +161,6 @@
     <t xml:space="preserve">Average number of jobs in normal center</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 74.091398 +/- 1.625701</t>
   </si>
   <si>
@@ -197,24 +194,33 @@
     <t xml:space="preserve"> 0.015625 +/- 0.021777</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of bypass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.000000 +/- 0.000000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Global response time</t>
   </si>
   <si>
-    <t xml:space="preserve">165.793473 +/- 1.765061</t>
+    <t xml:space="preserve"> 165.793473 +/- 1.765061</t>
   </si>
   <si>
     <t xml:space="preserve">Global Premium response time</t>
   </si>
   <si>
-    <t xml:space="preserve">141.137177 +/- 1.397107</t>
+    <t xml:space="preserve"> 141.137177 +/- 1.397107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Normal response time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 223.229941 +/- 4.647750</t>
   </si>
   <si>
     <t xml:space="preserve">Failure percentage</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.000000 +/- 0.000000</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rho in the digest center</t>
   </si>
   <si>
@@ -224,7 +230,7 @@
     <t xml:space="preserve">Rho in the normal center</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.974888 +/- 0.001283</t>
+    <t xml:space="preserve"> 0.973423 +/- 0.001269</t>
   </si>
   <si>
     <t xml:space="preserve">Rho in the premium center</t>
@@ -261,14 +267,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -285,13 +293,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -328,12 +349,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,13 +391,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -368,13 +405,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -437,7 +474,7 @@
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>232.945742</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -454,10 +491,6 @@
       <c r="C8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <f aca="false">143.158816+1.413922</f>
-        <v>144.572738</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -485,7 +518,7 @@
       <c r="A11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="2" t="n">
         <v>85.693088</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -575,7 +608,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="0" t="n">
-        <f aca="false">TRUNC(1/(B39/86400),6)</f>
+        <f aca="false">TRUNC(1/(B41/86400),6)</f>
         <v>3.026799</v>
       </c>
       <c r="C19" s="0" t="s">
@@ -587,7 +620,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="0" t="n">
-        <f aca="false">TRUNC(1/(B40/86400),6)</f>
+        <f aca="false">TRUNC(1/(B42/86400),6)</f>
         <v>1.297199</v>
       </c>
       <c r="C20" s="0" t="s">
@@ -599,7 +632,7 @@
         <v>41</v>
       </c>
       <c r="B21" s="0" t="n">
-        <f aca="false">TRUNC(1/(B41/86400),6)</f>
+        <f aca="false">TRUNC(1/(B43/86400),6)</f>
         <v>88.838877</v>
       </c>
       <c r="C21" s="0" t="s">
@@ -622,170 +655,179 @@
       <c r="A23" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="3" t="n">
+        <f aca="false">TRUNC((1/B19)*B7,6)</f>
+        <v>76.961087</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">TRUNC((1/B20)*B8,6)</f>
+        <v>111.297724</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="0" t="n">
         <f aca="false">TRUNC(1/B21*B9,6)</f>
         <v>5.077299</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">B41*B38</f>
+        <v>523.829295</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <f aca="false">B39*B36</f>
-        <v>523.829295</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">B42*B39</f>
+        <v>448.717885</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <f aca="false">B40*B37</f>
-        <v>448.717885</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <f aca="false">TRUNC(B43*B40,6)</f>
+        <v>0.005835</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <f aca="false">TRUNC(B41*B38,6)</f>
-        <v>0.005835</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <f aca="false">TRUNC(B6 + B7*B39/B2 + B8*B40/B2 + B9*B41/B2,6)</f>
-        <v>169.005948</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <f aca="false">TRUNC(B6 + B7*B41/B2 + B8*B42/B2 + B9*B43/B2,6)</f>
+        <v>169.005948</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <f aca="false">TRUNC(B6 + B8*B40/B2 + 148.418018*B37, 6)</f>
-        <v>99.124691</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <f aca="false">TRUNC(B6 + B8*B42/B4 + B9*B39, 6)</f>
+        <v>142.37553</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <f aca="false">TRUNC(B28/B20,6)</f>
-        <v>0.004498</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <f aca="false">TRUNC(B6 + B7*B41/B3 + B9*B38,6)</f>
+        <v>231.888938</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="0" t="n">
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <f aca="false">TRUNC(B28/B2,6)</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="0" t="n">
         <f aca="false">TRUNC(B14/B18,6)</f>
         <v>0.694444</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="0" t="n">
+      <c r="C34" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="4" t="n">
         <f aca="false">TRUNC(B15/(B19*50),6)</f>
         <v>0.972992</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="1" t="n">
+      <c r="C35" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="5" t="n">
         <f aca="false">TRUNC(B16/(B20*95),6)</f>
         <v>0.967196</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="1" t="n">
+      <c r="C36" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="5" t="n">
         <f aca="false">TRUNC(B17/(B21),6)</f>
         <v>0.844224</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>0.018351</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="C37" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>0.006737</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,8 +835,7 @@
         <v>74</v>
       </c>
       <c r="B38" s="0" t="n">
-        <f aca="false">TRUNC(6.144212/(1000000),6)</f>
-        <v>6E-006</v>
+        <v>0.018351</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,8 +843,7 @@
         <v>75</v>
       </c>
       <c r="B39" s="0" t="n">
-        <f aca="false">B3-B5*0.3</f>
-        <v>28545</v>
+        <v>0.006737</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -811,12 +851,8 @@
         <v>76</v>
       </c>
       <c r="B40" s="0" t="n">
-        <f aca="false">B4-B5*0.7</f>
-        <v>66605</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <f aca="false">B17/B21</f>
-        <v>0.84422498947167</v>
+        <f aca="false">TRUNC(6.144212/(1000000),6)</f>
+        <v>6E-006</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,6 +860,24 @@
         <v>77</v>
       </c>
       <c r="B41" s="0" t="n">
+        <f aca="false">B3-B5*0.3</f>
+        <v>28545</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <f aca="false">B4-B5*0.7</f>
+        <v>66605</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="0" t="n">
         <f aca="false">B26+B27</f>
         <v>972.54718</v>
       </c>
@@ -831,10 +885,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Pagina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -850,7 +904,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.51"/>
@@ -860,7 +914,7 @@
       <c r="A1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="5" t="n">
         <v>232.945742</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -871,7 +925,7 @@
       <c r="A2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="5" t="n">
         <v>85.693088</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -879,15 +933,15 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1"/>
+      <c r="B3" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Pagina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>